<commit_message>
Email adres gewijzigd voor Martijn Klomp moet Martijn Klomp2 zijn
</commit_message>
<xml_diff>
--- a/catalogusdata/BAG/Voorbeelden/Testdata VerblijfsObject T.xlsx
+++ b/catalogusdata/BAG/Voorbeelden/Testdata VerblijfsObject T.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="132">
   <si>
     <t>tabblad</t>
   </si>
@@ -200,24 +200,6 @@
     <t>http://purl.org/iso25964/skos-thes#{eigenschap}</t>
   </si>
   <si>
-    <t>Kop</t>
-  </si>
-  <si>
-    <t>Lijf</t>
-  </si>
-  <si>
-    <t>Poten</t>
-  </si>
-  <si>
-    <t>Een iets minder generiek, dan wel specifieker beest</t>
-  </si>
-  <si>
-    <t>Een behoorlijk specifiek beest</t>
-  </si>
-  <si>
-    <t>Deel van een beest</t>
-  </si>
-  <si>
     <t>testDomein</t>
   </si>
   <si>
@@ -242,15 +224,6 @@
     <t>Locatie geldigheid</t>
   </si>
   <si>
-    <t>1-1-2001 - 1-1-2017</t>
-  </si>
-  <si>
-    <t>1-1-2001 - 1-1-2016</t>
-  </si>
-  <si>
-    <t>1-1-2017 - 1-1-2018</t>
-  </si>
-  <si>
     <t>Collecties</t>
   </si>
   <si>
@@ -269,45 +242,6 @@
     <t>Concepten</t>
   </si>
   <si>
-    <t>Act</t>
-  </si>
-  <si>
-    <t>Een activiteit zo generiek dat het zijn gelijke niet kent</t>
-  </si>
-  <si>
-    <t>Een iets specifiekere activiteit</t>
-  </si>
-  <si>
-    <t>Een behoorlijk specifieke activiteit</t>
-  </si>
-  <si>
-    <t>Een activiteit zonder relaties</t>
-  </si>
-  <si>
-    <t>Norm</t>
-  </si>
-  <si>
-    <t>Een norm zo generiek dat het zijn gelijke niet kent</t>
-  </si>
-  <si>
-    <t>Een iets specifiekere norm</t>
-  </si>
-  <si>
-    <t>Een behoorlijk specifieke norm</t>
-  </si>
-  <si>
-    <t>Een norm zonder relaties</t>
-  </si>
-  <si>
-    <t>Een object zo generiek dat het zijn gelijke niet kent</t>
-  </si>
-  <si>
-    <t>Een object zonder relaties</t>
-  </si>
-  <si>
-    <t>Object</t>
-  </si>
-  <si>
     <t>rdf</t>
   </si>
   <si>
@@ -351,87 +285,6 @@
   </si>
   <si>
     <t>Bronnen</t>
-  </si>
-  <si>
-    <t>Beest</t>
-  </si>
-  <si>
-    <t>GeneriekBeest</t>
-  </si>
-  <si>
-    <t>Een beest dat duidelijk anders is dan GeneriekBeest</t>
-  </si>
-  <si>
-    <t>Een beest gerelateerd aan een GeneriekBeest</t>
-  </si>
-  <si>
-    <t>SpecifiekBeest</t>
-  </si>
-  <si>
-    <t>NogSpecifiekerBeest</t>
-  </si>
-  <si>
-    <t>AnderBeest</t>
-  </si>
-  <si>
-    <t>Een beest dat specifieker is dan AnderBeest</t>
-  </si>
-  <si>
-    <t>AnderSpecifiekBeest</t>
-  </si>
-  <si>
-    <t>SingleBeest</t>
-  </si>
-  <si>
-    <t>GerelateerdBeest</t>
-  </si>
-  <si>
-    <t>GeneriekeActiviteit</t>
-  </si>
-  <si>
-    <t>GeneriekeNorm</t>
-  </si>
-  <si>
-    <t>GeneriekObject</t>
-  </si>
-  <si>
-    <t>SpecifiekeActiviteit</t>
-  </si>
-  <si>
-    <t>SpecifiekeNorm</t>
-  </si>
-  <si>
-    <t>SingleActiviteit</t>
-  </si>
-  <si>
-    <t>SingleNorm</t>
-  </si>
-  <si>
-    <t>SingleObject</t>
-  </si>
-  <si>
-    <t>NogSpecifiekereActiviteit</t>
-  </si>
-  <si>
-    <t>NogSpecifiekereNorm</t>
-  </si>
-  <si>
-    <t>NogSpecifiekerObject</t>
-  </si>
-  <si>
-    <t>SpecifiekObject</t>
-  </si>
-  <si>
-    <t>Een iets specifieker object</t>
-  </si>
-  <si>
-    <t>Een behoorlijk specifiek object</t>
-  </si>
-  <si>
-    <t>Een beest dat geen relaties heeft. Zielig hè?</t>
-  </si>
-  <si>
-    <t>Deel van een beest, het hoofd zeg maar</t>
   </si>
   <si>
     <t>Waardelijsten</t>
@@ -559,6 +412,30 @@
   </si>
   <si>
     <t>2. Is er binnen de ruimte sprake van aaneengesloten samenhangend gebruik?</t>
+  </si>
+  <si>
+    <t>Pand_Vraag1</t>
+  </si>
+  <si>
+    <t>Pand_Vraag2</t>
+  </si>
+  <si>
+    <t>Pand_Vraag3</t>
+  </si>
+  <si>
+    <t>Pand_Vraag4</t>
+  </si>
+  <si>
+    <t>Pand_Vraag5</t>
+  </si>
+  <si>
+    <t>Pand_Vraag6</t>
+  </si>
+  <si>
+    <t>Pand_Vraag7</t>
+  </si>
+  <si>
+    <t>Pand_Vraag8</t>
   </si>
 </sst>
 </file>
@@ -638,7 +515,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
@@ -654,7 +531,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1054,7 +930,7 @@
         <v>27</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>107</v>
+        <v>85</v>
       </c>
       <c r="E5" t="s">
         <v>19</v>
@@ -1082,156 +958,156 @@
         <v>8</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>97</v>
+        <v>75</v>
       </c>
       <c r="E7" t="s">
-        <v>94</v>
+        <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="B8" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="C8" t="s">
         <v>4</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>138</v>
+        <v>89</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="B9" t="s">
-        <v>98</v>
+        <v>76</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>100</v>
+        <v>78</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="B10" t="s">
         <v>34</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>139</v>
+        <v>90</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="B11" t="s">
         <v>41</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>140</v>
+        <v>91</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="B12" t="s">
         <v>45</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>141</v>
+        <v>92</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="B13" t="s">
         <v>48</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>142</v>
+        <v>93</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="B14" t="s">
         <v>51</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>143</v>
+        <v>94</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="B15" t="s">
         <v>54</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>144</v>
+        <v>95</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="B16" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="C16" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>145</v>
+        <v>96</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="B17" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>138</v>
+        <v>89</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>136</v>
+        <v>87</v>
       </c>
       <c r="B18" t="s">
-        <v>137</v>
+        <v>88</v>
       </c>
       <c r="C18" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>146</v>
+        <v>97</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>136</v>
+        <v>87</v>
       </c>
       <c r="B19" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>145</v>
+        <v>96</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>108</v>
+        <v>86</v>
       </c>
       <c r="B20" t="s">
         <v>34</v>
@@ -1240,18 +1116,18 @@
         <v>4</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>139</v>
+        <v>90</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>108</v>
+        <v>86</v>
       </c>
       <c r="B21" t="s">
-        <v>98</v>
+        <v>76</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>106</v>
+        <v>84</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -1383,24 +1259,24 @@
     </row>
     <row r="2" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>98</v>
+        <v>76</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>94</v>
+        <v>72</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>95</v>
+        <v>73</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>96</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="B3" t="s">
         <v>10</v>
@@ -1420,10 +1296,10 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="B4" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="C4" t="s">
         <v>11</v>
@@ -1440,7 +1316,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="B5" t="s">
         <v>25</v>
@@ -1460,7 +1336,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="B6" t="s">
         <v>28</v>
@@ -1480,7 +1356,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="B7" t="s">
         <v>33</v>
@@ -1497,7 +1373,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="B8" t="s">
         <v>38</v>
@@ -1514,7 +1390,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="B9" t="s">
         <v>34</v>
@@ -1531,7 +1407,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="B10" t="s">
         <v>41</v>
@@ -1548,7 +1424,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="B11" t="s">
         <v>45</v>
@@ -1565,7 +1441,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="B12" t="s">
         <v>48</v>
@@ -1582,7 +1458,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="B13" t="s">
         <v>51</v>
@@ -1599,7 +1475,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="B14" t="s">
         <v>54</v>
@@ -1616,27 +1492,27 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="B15" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="C15" t="s">
         <v>19</v>
       </c>
       <c r="D15" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="E15" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="C16" s="9" t="s">
         <v>18</v>
@@ -1650,10 +1526,10 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="C17" s="9" t="s">
         <v>11</v>
@@ -1667,7 +1543,7 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="B18" s="9" t="s">
         <v>28</v>
@@ -1684,62 +1560,62 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="C19" s="9" t="s">
         <v>19</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E19" s="9" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="F19" s="6"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="C20" s="9" t="s">
         <v>19</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="E20" s="9" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="C21" s="9" t="s">
         <v>11</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="E21" s="9" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
-        <v>136</v>
+        <v>87</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>137</v>
+        <v>88</v>
       </c>
       <c r="C22" s="9" t="s">
         <v>18</v>
@@ -1753,10 +1629,10 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
-        <v>136</v>
+        <v>87</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>137</v>
+        <v>88</v>
       </c>
       <c r="C23" s="9" t="s">
         <v>11</v>
@@ -1770,7 +1646,7 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
-        <v>136</v>
+        <v>87</v>
       </c>
       <c r="B24" s="9" t="s">
         <v>28</v>
@@ -1787,41 +1663,41 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
-        <v>136</v>
+        <v>87</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="C25" s="9" t="s">
         <v>19</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="E25" s="9" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
-        <v>136</v>
+        <v>87</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="C26" s="9" t="s">
         <v>11</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="E26" s="9" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
-        <v>108</v>
+        <v>86</v>
       </c>
       <c r="B27" s="9" t="s">
         <v>34</v>
@@ -1838,7 +1714,7 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
-        <v>108</v>
+        <v>86</v>
       </c>
       <c r="B28" s="9" t="s">
         <v>34</v>
@@ -1855,24 +1731,24 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="s">
-        <v>108</v>
+        <v>86</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>98</v>
+        <v>76</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>94</v>
+        <v>72</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>95</v>
+        <v>73</v>
       </c>
       <c r="E29" s="9" t="s">
-        <v>96</v>
+        <v>74</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="s">
-        <v>108</v>
+        <v>86</v>
       </c>
       <c r="B30" s="9" t="s">
         <v>10</v>
@@ -1889,7 +1765,7 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="9" t="s">
-        <v>108</v>
+        <v>86</v>
       </c>
       <c r="B31" s="9" t="s">
         <v>28</v>
@@ -1911,7 +1787,7 @@
       <c r="D42" s="9"/>
       <c r="E42" s="9"/>
     </row>
-    <row r="52" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52"/>
       <c r="B52"/>
       <c r="C52"/>
@@ -1926,11 +1802,11 @@
       <c r="E56" s="9"/>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A57" s="12"/>
-      <c r="B57" s="12"/>
-      <c r="C57" s="12"/>
-      <c r="D57" s="12"/>
-      <c r="E57" s="12"/>
+      <c r="A57" s="11"/>
+      <c r="B57" s="11"/>
+      <c r="C57" s="11"/>
+      <c r="D57" s="11"/>
+      <c r="E57" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1940,10 +1816,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N44"/>
+  <dimension ref="A1:U42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1961,15 +1837,15 @@
     <col min="14" max="14" width="32" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>98</v>
+        <v>76</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>10</v>
@@ -1987,7 +1863,7 @@
         <v>34</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="J1" s="4" t="s">
         <v>41</v>
@@ -2005,21 +1881,21 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
-        <v>148</v>
+        <v>99</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>171</v>
+        <v>122</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>27</v>
       </c>
       <c r="E2" t="s">
-        <v>152</v>
+        <v>103</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>149</v>
+        <v>100</v>
       </c>
       <c r="G2" s="9" t="s">
         <v>27</v>
@@ -2035,24 +1911,24 @@
       </c>
       <c r="M2" s="5"/>
       <c r="N2" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>148</v>
+        <v>99</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>171</v>
+        <v>122</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>27</v>
       </c>
       <c r="E3" t="s">
-        <v>152</v>
+        <v>103</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>149</v>
+        <v>100</v>
       </c>
       <c r="G3" s="9" t="s">
         <v>27</v>
@@ -2068,155 +1944,155 @@
       </c>
       <c r="M3" s="5"/>
       <c r="N3" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" s="9" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" s="9" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>153</v>
+        <v>104</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>172</v>
+        <v>123</v>
       </c>
       <c r="D4" s="5"/>
       <c r="E4" t="s">
-        <v>152</v>
-      </c>
-      <c r="F4" s="14" t="s">
-        <v>154</v>
+        <v>103</v>
+      </c>
+      <c r="F4" s="13" t="s">
+        <v>105</v>
       </c>
       <c r="H4"/>
       <c r="I4" s="10"/>
       <c r="K4" s="5"/>
       <c r="M4" s="5"/>
       <c r="N4" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" s="9" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" s="9" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>156</v>
+        <v>107</v>
       </c>
       <c r="D5" s="5"/>
       <c r="E5" t="s">
-        <v>152</v>
-      </c>
-      <c r="F5" s="14" t="s">
-        <v>164</v>
+        <v>103</v>
+      </c>
+      <c r="F5" s="13" t="s">
+        <v>115</v>
       </c>
       <c r="H5"/>
       <c r="I5" s="10"/>
       <c r="K5" s="5"/>
       <c r="M5" s="5"/>
       <c r="N5" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" s="9" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" s="9" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>156</v>
+        <v>107</v>
       </c>
       <c r="D6" s="5"/>
       <c r="E6" t="s">
-        <v>152</v>
-      </c>
-      <c r="F6" s="14" t="s">
-        <v>164</v>
+        <v>103</v>
+      </c>
+      <c r="F6" s="13" t="s">
+        <v>115</v>
       </c>
       <c r="H6"/>
       <c r="I6" s="10"/>
       <c r="K6" s="5"/>
       <c r="M6" s="5"/>
       <c r="N6" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" s="9" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" s="9" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
-        <v>156</v>
+        <v>107</v>
       </c>
       <c r="D7" s="5"/>
       <c r="E7" t="s">
-        <v>152</v>
-      </c>
-      <c r="F7" s="14" t="s">
-        <v>164</v>
+        <v>103</v>
+      </c>
+      <c r="F7" s="13" t="s">
+        <v>115</v>
       </c>
       <c r="H7"/>
       <c r="I7" s="10"/>
       <c r="K7" s="5"/>
       <c r="M7" s="5"/>
       <c r="N7" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" s="9" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" s="9" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
-        <v>156</v>
+        <v>107</v>
       </c>
       <c r="D8" s="5"/>
       <c r="E8" t="s">
-        <v>152</v>
-      </c>
-      <c r="F8" s="14" t="s">
-        <v>164</v>
+        <v>103</v>
+      </c>
+      <c r="F8" s="13" t="s">
+        <v>115</v>
       </c>
       <c r="H8"/>
       <c r="I8" s="10"/>
       <c r="K8" s="5"/>
       <c r="M8" s="5"/>
       <c r="N8" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" s="9" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" s="9" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
-        <v>156</v>
+        <v>107</v>
       </c>
       <c r="D9" s="5"/>
       <c r="E9" t="s">
-        <v>152</v>
-      </c>
-      <c r="F9" s="14" t="s">
-        <v>164</v>
+        <v>103</v>
+      </c>
+      <c r="F9" s="13" t="s">
+        <v>115</v>
       </c>
       <c r="H9"/>
       <c r="I9" s="10"/>
       <c r="K9" s="5"/>
       <c r="M9" s="5"/>
       <c r="N9" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" s="9" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" s="9" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
-        <v>156</v>
+        <v>107</v>
       </c>
       <c r="D10" s="5"/>
       <c r="E10" t="s">
-        <v>152</v>
-      </c>
-      <c r="F10" s="14" t="s">
-        <v>164</v>
+        <v>103</v>
+      </c>
+      <c r="F10" s="13" t="s">
+        <v>115</v>
       </c>
       <c r="H10"/>
       <c r="I10" s="10"/>
       <c r="K10" s="5"/>
       <c r="M10" s="5"/>
       <c r="N10" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" s="9" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" s="9" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
         <v>27</v>
       </c>
       <c r="D11" s="5"/>
       <c r="E11" t="s">
-        <v>152</v>
-      </c>
-      <c r="F11" s="14" t="s">
-        <v>164</v>
+        <v>103</v>
+      </c>
+      <c r="F11" s="13" t="s">
+        <v>115</v>
       </c>
       <c r="H11"/>
       <c r="I11" s="10"/>
@@ -2224,509 +2100,76 @@
       <c r="M11" s="5"/>
       <c r="N11"/>
     </row>
-    <row r="12" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
-        <v>157</v>
+        <v>108</v>
       </c>
       <c r="D12" s="5"/>
       <c r="E12"/>
-      <c r="F12" s="14"/>
+      <c r="F12" s="13"/>
       <c r="H12"/>
       <c r="I12" s="10"/>
       <c r="K12" s="5"/>
       <c r="M12" s="5"/>
       <c r="N12"/>
     </row>
-    <row r="13" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13"/>
+      <c r="B13"/>
+      <c r="C13"/>
       <c r="D13" s="5"/>
-      <c r="E13"/>
-      <c r="F13" s="14"/>
+      <c r="E13" s="3"/>
+      <c r="F13"/>
+      <c r="G13"/>
       <c r="H13"/>
-      <c r="I13" s="10"/>
+      <c r="I13"/>
+      <c r="J13" s="5"/>
       <c r="K13" s="5"/>
+      <c r="L13"/>
       <c r="M13" s="5"/>
       <c r="N13"/>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>113</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="E14" t="s">
-        <v>64</v>
-      </c>
-      <c r="H14" t="s">
-        <v>102</v>
-      </c>
-      <c r="I14" t="s">
-        <v>72</v>
-      </c>
-      <c r="J14" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="K14" s="5" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>114</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="E15" t="s">
-        <v>64</v>
-      </c>
-      <c r="I15" t="s">
-        <v>73</v>
-      </c>
-      <c r="J15" s="5" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>58</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>135</v>
-      </c>
-      <c r="E16" t="s">
-        <v>64</v>
-      </c>
-      <c r="I16" s="10">
-        <v>36892</v>
-      </c>
-      <c r="L16" t="s">
-        <v>110</v>
-      </c>
+      <c r="O13"/>
+      <c r="P13"/>
+      <c r="Q13"/>
+      <c r="R13"/>
+      <c r="S13"/>
+      <c r="T13"/>
+      <c r="U13"/>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="E14" s="3"/>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="E15" s="3"/>
+      <c r="N15" s="5"/>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="E16" s="3"/>
       <c r="N16" s="5"/>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>109</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="E17" t="s">
-        <v>64</v>
-      </c>
-      <c r="I17" s="10">
-        <v>1</v>
-      </c>
-      <c r="M17" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="N17" s="5"/>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>59</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="E18" t="s">
-        <v>64</v>
-      </c>
-      <c r="I18" s="10">
-        <v>36892</v>
-      </c>
-      <c r="L18" t="s">
-        <v>110</v>
-      </c>
-      <c r="N18" s="5"/>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>60</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="E19" t="s">
-        <v>64</v>
-      </c>
-      <c r="I19" s="10">
-        <v>36892</v>
-      </c>
-      <c r="L19" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="N19" s="5"/>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A20" s="8" t="s">
-        <v>115</v>
-      </c>
-      <c r="B20" s="8"/>
-      <c r="C20" s="8"/>
-      <c r="D20" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="E20" t="s">
-        <v>64</v>
-      </c>
-      <c r="I20" s="10">
-        <v>42736</v>
-      </c>
-      <c r="K20" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="L20" s="5"/>
-      <c r="N20" s="5" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A21" s="8" t="s">
-        <v>117</v>
-      </c>
-      <c r="B21" s="8"/>
-      <c r="C21" s="8"/>
-      <c r="D21" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="E21" t="s">
-        <v>64</v>
-      </c>
-      <c r="I21" s="10">
-        <v>42736</v>
-      </c>
-      <c r="J21" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="N21" s="5"/>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A22" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="B22" s="8"/>
-      <c r="C22" s="8"/>
-      <c r="D22" s="5" t="s">
-        <v>134</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="I22" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="N22" s="5" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>119</v>
-      </c>
-      <c r="C23" s="8"/>
-      <c r="D23" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="E23" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="H23" s="6"/>
-      <c r="I23" s="11">
-        <v>36892</v>
-      </c>
-      <c r="N23" s="5" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A24" s="9" t="s">
-        <v>120</v>
-      </c>
-      <c r="B24" s="9"/>
-      <c r="C24" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="D24" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="E24" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="F24" s="9"/>
-      <c r="G24" s="9"/>
-      <c r="I24" s="10"/>
-      <c r="J24" s="9"/>
-      <c r="K24" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="L24" s="9"/>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>123</v>
-      </c>
-      <c r="C25" t="s">
-        <v>81</v>
-      </c>
-      <c r="D25" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="E25" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="F25" s="9"/>
-      <c r="G25" s="9"/>
-      <c r="I25" s="10"/>
-      <c r="J25" s="9" t="s">
-        <v>120</v>
-      </c>
-      <c r="K25" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="L25" s="9"/>
-      <c r="N25" s="9"/>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>128</v>
-      </c>
-      <c r="C26" t="s">
-        <v>81</v>
-      </c>
-      <c r="D26" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="E26" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="F26" s="9"/>
-      <c r="G26" s="9"/>
-      <c r="I26" s="10"/>
-      <c r="J26" s="9" t="s">
-        <v>123</v>
-      </c>
-      <c r="L26" s="9"/>
-      <c r="N26" s="9"/>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>125</v>
-      </c>
-      <c r="C27" t="s">
-        <v>81</v>
-      </c>
-      <c r="D27" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="E27" s="7" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A28" s="9" t="s">
-        <v>121</v>
-      </c>
-      <c r="B28" s="9"/>
-      <c r="C28" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="D28" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="E28" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="F28" s="9"/>
-      <c r="G28" s="9"/>
-      <c r="I28" s="10"/>
-      <c r="J28" s="9"/>
-      <c r="K28" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="L28" s="9"/>
-      <c r="N28" s="6"/>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>124</v>
-      </c>
-      <c r="C29" t="s">
-        <v>86</v>
-      </c>
-      <c r="D29" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="E29" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="F29" s="9"/>
-      <c r="G29" s="9"/>
-      <c r="I29" s="10"/>
-      <c r="J29" s="9" t="s">
-        <v>121</v>
-      </c>
-      <c r="K29" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="L29" s="9"/>
-      <c r="N29" s="5"/>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>129</v>
-      </c>
-      <c r="C30" t="s">
-        <v>86</v>
-      </c>
-      <c r="D30" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="E30" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="F30" s="9"/>
-      <c r="G30" s="9"/>
-      <c r="I30" s="10"/>
-      <c r="J30" s="9" t="s">
-        <v>124</v>
-      </c>
-      <c r="L30" s="9"/>
-      <c r="N30" s="5"/>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>126</v>
-      </c>
-      <c r="C31" t="s">
-        <v>86</v>
-      </c>
-      <c r="D31" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="E31" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="N31" s="5"/>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A32" s="9" t="s">
-        <v>122</v>
-      </c>
-      <c r="B32" s="9"/>
-      <c r="C32" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="D32" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="E32" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="F32" s="9"/>
-      <c r="G32" s="9"/>
-      <c r="I32" s="10"/>
-      <c r="J32" s="9"/>
-      <c r="K32" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="L32" s="9"/>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>131</v>
-      </c>
-      <c r="C33" t="s">
-        <v>93</v>
-      </c>
-      <c r="D33" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="E33" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="F33" s="9"/>
-      <c r="G33" s="9"/>
-      <c r="I33" s="10"/>
-      <c r="J33" s="9" t="s">
-        <v>122</v>
-      </c>
-      <c r="K33" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="L33" s="9"/>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>130</v>
-      </c>
-      <c r="C34" t="s">
-        <v>93</v>
-      </c>
-      <c r="D34" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="E34" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="F34" s="9"/>
-      <c r="G34" s="9"/>
-      <c r="I34" s="10"/>
-      <c r="J34" s="9" t="s">
-        <v>131</v>
-      </c>
-      <c r="L34" s="9"/>
-    </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>127</v>
-      </c>
-      <c r="C35" t="s">
-        <v>93</v>
-      </c>
-      <c r="D35" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="E35" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="N35" s="5"/>
-    </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="E38" s="3"/>
-    </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="E39" s="3"/>
-    </row>
-    <row r="40" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E40" s="3"/>
-      <c r="N40" s="5"/>
-    </row>
-    <row r="41" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E41" s="3"/>
-      <c r="N41" s="5"/>
-    </row>
-    <row r="42" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="8"/>
-      <c r="B42" s="8"/>
-      <c r="C42" s="8"/>
-      <c r="E42" s="3"/>
-    </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A43" s="13"/>
-      <c r="B43" s="13"/>
-      <c r="C43" s="13"/>
-      <c r="E43" s="7"/>
-      <c r="H43" s="6"/>
-      <c r="I43" s="6"/>
-    </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A44" s="8"/>
-      <c r="B44" s="8"/>
-      <c r="C44" s="8"/>
-      <c r="E44" s="3"/>
-    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="8"/>
+      <c r="B17" s="8"/>
+      <c r="C17" s="8"/>
+      <c r="E17" s="3"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="12"/>
+      <c r="B18" s="12"/>
+      <c r="C18" s="12"/>
+      <c r="E18" s="7"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="6"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="8"/>
+      <c r="B19" s="8"/>
+      <c r="C19" s="8"/>
+      <c r="E19" s="3"/>
+    </row>
+    <row r="40" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="41" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="42" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2737,8 +2180,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2750,27 +2193,27 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>147</v>
+        <v>98</v>
       </c>
       <c r="B2" t="s">
-        <v>152</v>
+        <v>103</v>
       </c>
       <c r="C2" t="s">
         <v>27</v>
@@ -2779,152 +2222,237 @@
         <v>42736</v>
       </c>
       <c r="E2" t="s">
-        <v>148</v>
+        <v>99</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>147</v>
+        <v>98</v>
       </c>
       <c r="B3" t="s">
-        <v>152</v>
+        <v>103</v>
       </c>
       <c r="D3" s="10">
-        <v>42737</v>
+        <v>42736</v>
       </c>
       <c r="E3" t="s">
-        <v>153</v>
+        <v>104</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>147</v>
+        <v>98</v>
       </c>
       <c r="B4" t="s">
-        <v>152</v>
+        <v>103</v>
       </c>
       <c r="D4" s="10">
-        <v>42738</v>
+        <v>42736</v>
       </c>
       <c r="E4" t="s">
-        <v>156</v>
+        <v>107</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>147</v>
+        <v>98</v>
       </c>
       <c r="B5" t="s">
-        <v>152</v>
+        <v>103</v>
       </c>
       <c r="D5" s="10">
-        <v>42739</v>
+        <v>42736</v>
       </c>
       <c r="E5" t="s">
-        <v>157</v>
+        <v>108</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>147</v>
+        <v>98</v>
       </c>
       <c r="B6" t="s">
-        <v>152</v>
+        <v>103</v>
       </c>
       <c r="D6" s="10">
-        <v>42740</v>
+        <v>42736</v>
       </c>
       <c r="E6" t="s">
-        <v>158</v>
+        <v>109</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>147</v>
+        <v>98</v>
       </c>
       <c r="B7" t="s">
-        <v>152</v>
+        <v>103</v>
       </c>
       <c r="D7" s="10">
-        <v>42741</v>
+        <v>42736</v>
       </c>
       <c r="E7" t="s">
-        <v>159</v>
+        <v>110</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>147</v>
+        <v>98</v>
       </c>
       <c r="B8" t="s">
-        <v>152</v>
+        <v>103</v>
       </c>
       <c r="D8" s="10">
-        <v>42742</v>
+        <v>42736</v>
       </c>
       <c r="E8" t="s">
-        <v>160</v>
+        <v>111</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>147</v>
+        <v>98</v>
       </c>
       <c r="B9" t="s">
-        <v>152</v>
+        <v>103</v>
       </c>
       <c r="D9" s="10">
-        <v>42743</v>
+        <v>42736</v>
       </c>
       <c r="E9" t="s">
-        <v>161</v>
+        <v>112</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>147</v>
+        <v>98</v>
       </c>
       <c r="B10" t="s">
-        <v>152</v>
+        <v>103</v>
       </c>
       <c r="D10" s="10">
-        <v>42744</v>
+        <v>42736</v>
       </c>
       <c r="E10" t="s">
-        <v>162</v>
+        <v>113</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>163</v>
-      </c>
-      <c r="D11" s="10"/>
+        <v>114</v>
+      </c>
+      <c r="B11" t="s">
+        <v>103</v>
+      </c>
+      <c r="D11" s="10">
+        <v>42736</v>
+      </c>
+      <c r="E11" t="s">
+        <v>124</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D12" s="10"/>
+      <c r="A12" t="s">
+        <v>114</v>
+      </c>
+      <c r="B12" t="s">
+        <v>103</v>
+      </c>
+      <c r="D12" s="10">
+        <v>42736</v>
+      </c>
+      <c r="E12" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D13" s="10"/>
+      <c r="A13" t="s">
+        <v>114</v>
+      </c>
+      <c r="B13" t="s">
+        <v>103</v>
+      </c>
+      <c r="D13" s="10">
+        <v>42736</v>
+      </c>
+      <c r="E13" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D14" s="10"/>
+      <c r="A14" t="s">
+        <v>114</v>
+      </c>
+      <c r="B14" t="s">
+        <v>103</v>
+      </c>
+      <c r="D14" s="10">
+        <v>42736</v>
+      </c>
+      <c r="E14" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D15" s="10"/>
+      <c r="A15" t="s">
+        <v>114</v>
+      </c>
+      <c r="B15" t="s">
+        <v>103</v>
+      </c>
+      <c r="D15" s="10">
+        <v>42736</v>
+      </c>
+      <c r="E15" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D16" s="10"/>
-    </row>
-    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D17" s="10"/>
-    </row>
-    <row r="18" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D18" s="10"/>
-    </row>
-    <row r="19" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>114</v>
+      </c>
+      <c r="B16" t="s">
+        <v>103</v>
+      </c>
+      <c r="D16" s="10">
+        <v>42736</v>
+      </c>
+      <c r="E16" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>114</v>
+      </c>
+      <c r="B17" t="s">
+        <v>103</v>
+      </c>
+      <c r="D17" s="10">
+        <v>42736</v>
+      </c>
+      <c r="E17" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>114</v>
+      </c>
+      <c r="B18" t="s">
+        <v>103</v>
+      </c>
+      <c r="D18" s="10">
+        <v>42736</v>
+      </c>
+      <c r="E18" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D19" s="10"/>
     </row>
-    <row r="20" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D20" s="10"/>
     </row>
   </sheetData>
@@ -2950,27 +2478,27 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>137</v>
+        <v>88</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>136</v>
+        <v>87</v>
       </c>
       <c r="B2" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="D2" t="s">
-        <v>99</v>
+        <v>77</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -3015,7 +2543,7 @@
         <v>34</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>98</v>
+        <v>76</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>10</v>
@@ -3026,30 +2554,30 @@
     </row>
     <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>102</v>
+        <v>80</v>
       </c>
       <c r="B2" t="s">
-        <v>103</v>
+        <v>81</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>104</v>
+        <v>82</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>101</v>
+        <v>79</v>
       </c>
       <c r="B3" t="s">
-        <v>103</v>
+        <v>81</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>105</v>
+        <v>83</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>